<commit_message>
made PT test program
</commit_message>
<xml_diff>
--- a/Project2Main/Phototransistor_Readings.xlsx
+++ b/Project2Main/Phototransistor_Readings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni\MECHENG_706\MECHENG706\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni\MECHENG_706\MECHENG706\Project2Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1AC60D-394E-4937-AAEE-D0BC4997FD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0646B5B1-25A0-41C6-8397-73B710C4CD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,47 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>-30°</t>
+  </si>
+  <si>
+    <t>-15°</t>
+  </si>
+  <si>
+    <t>0°</t>
+  </si>
+  <si>
+    <t>15°</t>
+  </si>
+  <si>
+    <t>30°</t>
+  </si>
+  <si>
+    <t>75mm</t>
+  </si>
+  <si>
+    <t>100mm</t>
+  </si>
+  <si>
+    <t>150mm</t>
+  </si>
+  <si>
+    <t>200mm</t>
+  </si>
+  <si>
     <r>
-      <t>40k</t>
+      <t>300k</t>
     </r>
     <r>
       <rPr>
@@ -39,45 +78,6 @@
       </rPr>
       <t>Ω</t>
     </r>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>-30°</t>
-  </si>
-  <si>
-    <t>-15°</t>
-  </si>
-  <si>
-    <t>0°</t>
-  </si>
-  <si>
-    <t>15°</t>
-  </si>
-  <si>
-    <t>30°</t>
-  </si>
-  <si>
-    <t>75mm</t>
-  </si>
-  <si>
-    <t>100mm</t>
-  </si>
-  <si>
-    <t>150mm</t>
-  </si>
-  <si>
-    <t>200mm</t>
   </si>
 </sst>
 </file>
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -281,10 +281,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -566,266 +564,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="10"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3"/>
       <c r="B9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="2"/>
       <c r="B11" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="2"/>
       <c r="B12" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="9"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="13" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="2"/>
       <c r="B15" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="17" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
       <c r="B20" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="21" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="G22" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
debugged pt_test, got some values
</commit_message>
<xml_diff>
--- a/Project2Main/Phototransistor_Readings.xlsx
+++ b/Project2Main/Phototransistor_Readings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni\MECHENG_706\MECHENG706\Project2Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0646B5B1-25A0-41C6-8397-73B710C4CD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA86722-B622-446E-AADE-821FB3935C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9920" yWindow="0" windowWidth="10160" windowHeight="12693" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>P1</t>
   </si>
@@ -42,15 +42,9 @@
     <t>-30°</t>
   </si>
   <si>
-    <t>-15°</t>
-  </si>
-  <si>
     <t>0°</t>
   </si>
   <si>
-    <t>15°</t>
-  </si>
-  <si>
     <t>30°</t>
   </si>
   <si>
@@ -66,8 +60,14 @@
     <t>200mm</t>
   </si>
   <si>
+    <t>-60°</t>
+  </si>
+  <si>
+    <t>60°</t>
+  </si>
+  <si>
     <r>
-      <t>300k</t>
+      <t>20M</t>
     </r>
     <r>
       <rPr>
@@ -78,6 +78,9 @@
       </rPr>
       <t>Ω</t>
     </r>
+  </si>
+  <si>
+    <t>PT1 &amp; PT2 seem okay, PT3 &amp; PT4 less so</t>
   </si>
 </sst>
 </file>
@@ -564,9 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -576,227 +581,392 @@
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="6">
+        <v>976.44</v>
+      </c>
+      <c r="D2" s="6">
+        <v>980.76</v>
+      </c>
+      <c r="E2" s="6">
+        <v>992.2</v>
+      </c>
+      <c r="F2" s="6">
+        <v>995.1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="C3" s="7">
+        <v>946.5</v>
+      </c>
+      <c r="D3" s="7">
+        <v>961.28</v>
+      </c>
+      <c r="E3" s="7">
+        <v>976.32</v>
+      </c>
+      <c r="F3" s="7">
+        <v>983.66</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="C4" s="7">
+        <v>994.4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1000.54</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1006.28</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1008.06</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="8">
+        <v>1020.36</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1019.72</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1018.48</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1020.28</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="6">
+        <v>950.08</v>
+      </c>
+      <c r="D6" s="6">
+        <v>975.46</v>
+      </c>
+      <c r="E6" s="6">
+        <v>987.28</v>
+      </c>
+      <c r="F6" s="6">
+        <v>997</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="7">
+        <v>846.12</v>
+      </c>
+      <c r="D7" s="7">
+        <v>876.18</v>
+      </c>
+      <c r="E7" s="7">
+        <v>882.32</v>
+      </c>
+      <c r="F7" s="7">
+        <v>919.8</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="C8" s="7">
+        <v>958.62</v>
+      </c>
+      <c r="D8" s="7">
+        <v>976.68</v>
+      </c>
+      <c r="E8" s="7">
+        <v>968.92</v>
+      </c>
+      <c r="F8" s="7">
+        <v>983.66</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3"/>
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="8">
+        <v>1019.2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1020.02</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1019.78</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1018.36</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="6">
+        <v>966.74</v>
+      </c>
+      <c r="D10" s="6">
+        <v>978.36</v>
+      </c>
+      <c r="E10" s="6">
+        <v>988.44</v>
+      </c>
+      <c r="F10" s="6">
+        <v>994.98</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="2"/>
       <c r="B11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="C11" s="7">
+        <v>141.44</v>
+      </c>
+      <c r="D11" s="7">
+        <v>147.62</v>
+      </c>
+      <c r="E11" s="7">
+        <v>271.3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>468.16</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="2"/>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="7"/>
+      <c r="C12" s="7">
+        <v>744.08</v>
+      </c>
+      <c r="D12" s="7">
+        <v>744.26</v>
+      </c>
+      <c r="E12" s="9">
+        <v>748.54</v>
+      </c>
+      <c r="F12" s="7">
+        <v>816.14</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="C13" s="8">
+        <v>1020.42</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1020.06</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1020.54</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1017.92</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="C14" s="6">
+        <v>968.12</v>
+      </c>
+      <c r="D14" s="6">
+        <v>980.2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>989.5</v>
+      </c>
+      <c r="F14" s="6">
+        <v>995.2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="2"/>
       <c r="B15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="C15" s="7">
+        <v>118.24</v>
+      </c>
+      <c r="D15" s="7">
+        <v>127.68</v>
+      </c>
+      <c r="E15" s="7">
+        <v>140.18</v>
+      </c>
+      <c r="F15" s="7">
+        <v>151.28</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="C16" s="7">
+        <v>744.82</v>
+      </c>
+      <c r="D16" s="7">
+        <v>745.4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>744.48</v>
+      </c>
+      <c r="F16" s="7">
+        <v>743.96</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="C17" s="8">
+        <v>1019.44</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1019</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1020.02</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1019.96</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="C18" s="6">
+        <v>976.24</v>
+      </c>
+      <c r="D18" s="6">
+        <v>976.28</v>
+      </c>
+      <c r="E18" s="6">
+        <v>987.82</v>
+      </c>
+      <c r="F18" s="6">
+        <v>995.16</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="C19" s="7">
+        <v>112.46</v>
+      </c>
+      <c r="D19" s="7">
+        <v>123.68</v>
+      </c>
+      <c r="E19" s="7">
+        <v>138.38</v>
+      </c>
+      <c r="F19" s="7">
+        <v>150.5</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
       <c r="B20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="C20" s="7">
+        <v>744.7</v>
+      </c>
+      <c r="D20" s="7">
+        <v>744.62</v>
+      </c>
+      <c r="E20" s="7">
+        <v>744.52</v>
+      </c>
+      <c r="F20" s="7">
+        <v>744.24</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="C21" s="8">
+        <v>1020.48</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1020.54</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1020.32</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1020.32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>